<commit_message>
:zap: v2.1 project completed
</commit_message>
<xml_diff>
--- a/Node/webScrapping/espn_scrapper/IPL/Delhi Capitals/Ajinkya Rahane .xlsx
+++ b/Node/webScrapping/espn_scrapper/IPL/Delhi Capitals/Ajinkya Rahane .xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,42 +439,252 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve"> Nov 10 2020</v>
+        <v xml:space="preserve"> Oct 24 2020</v>
       </c>
       <c r="B2" t="str">
-        <v xml:space="preserve"> Dubai (DSC)</v>
+        <v xml:space="preserve"> Abu Dhabi</v>
       </c>
       <c r="C2" t="str">
-        <v>Mumbai won by 5 wickets (with 8 balls remaining)</v>
+        <v>KKR won by 59 runs</v>
       </c>
       <c r="D2" t="str">
         <v>Delhi Capitals</v>
       </c>
       <c r="E2" t="str">
-        <v>Mumbai Indians</v>
+        <v>Kolkata Knight Riders</v>
       </c>
       <c r="F2" t="str">
         <v xml:space="preserve">Ajinkya Rahane </v>
       </c>
       <c r="G2" t="str">
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <v>0</v>
+      </c>
+      <c r="K2" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v xml:space="preserve"> Nov 10 2020</v>
+      </c>
+      <c r="B3" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Mumbai won by 5 wickets (with 8 balls remaining)</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="F3" t="str">
+        <v xml:space="preserve">Ajinkya Rahane </v>
+      </c>
+      <c r="G3" t="str">
         <v>2</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H3" t="str">
         <v>4</v>
       </c>
-      <c r="I2" t="str">
-        <v>0</v>
-      </c>
-      <c r="J2" t="str">
-        <v>0</v>
-      </c>
-      <c r="K2" t="str">
+      <c r="I3" t="str">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <v>0</v>
+      </c>
+      <c r="K3" t="str">
         <v>50.00</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve"> Nov 2 2020</v>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Capitals won by 6 wickets (with 6 balls remaining)</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Royal Challengers Bangalore</v>
+      </c>
+      <c r="F4" t="str">
+        <v xml:space="preserve">Ajinkya Rahane </v>
+      </c>
+      <c r="G4" t="str">
+        <v>60</v>
+      </c>
+      <c r="H4" t="str">
+        <v>46</v>
+      </c>
+      <c r="I4" t="str">
+        <v>5</v>
+      </c>
+      <c r="J4" t="str">
+        <v>1</v>
+      </c>
+      <c r="K4" t="str">
+        <v>130.43</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve"> Oct 11 2020</v>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Mumbai won by 5 wickets (with 2 balls remaining)</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="F5" t="str">
+        <v xml:space="preserve">Ajinkya Rahane </v>
+      </c>
+      <c r="G5" t="str">
+        <v>15</v>
+      </c>
+      <c r="H5" t="str">
+        <v>15</v>
+      </c>
+      <c r="I5" t="str">
+        <v>3</v>
+      </c>
+      <c r="J5" t="str">
+        <v>0</v>
+      </c>
+      <c r="K5" t="str">
+        <v>100.00</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve"> Nov 5 2020</v>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Mumbai won by 57 runs</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="F6" t="str">
+        <v xml:space="preserve">Ajinkya Rahane </v>
+      </c>
+      <c r="G6" t="str">
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <v>3</v>
+      </c>
+      <c r="I6" t="str">
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <v>0</v>
+      </c>
+      <c r="K6" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve"> Oct 17 2020</v>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve"> Sharjah</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Capitals won by 5 wickets (with 1 ball remaining)</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="F7" t="str">
+        <v xml:space="preserve">Ajinkya Rahane </v>
+      </c>
+      <c r="G7" t="str">
+        <v>8</v>
+      </c>
+      <c r="H7" t="str">
+        <v>10</v>
+      </c>
+      <c r="I7" t="str">
+        <v>1</v>
+      </c>
+      <c r="J7" t="str">
+        <v>0</v>
+      </c>
+      <c r="K7" t="str">
+        <v>80.00</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve"> Oct 14 2020</v>
+      </c>
+      <c r="B8" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Capitals won by 13 runs</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Rajasthan Royals</v>
+      </c>
+      <c r="F8" t="str">
+        <v xml:space="preserve">Ajinkya Rahane </v>
+      </c>
+      <c r="G8" t="str">
+        <v>2</v>
+      </c>
+      <c r="H8" t="str">
+        <v>9</v>
+      </c>
+      <c r="I8" t="str">
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
+        <v>0</v>
+      </c>
+      <c r="K8" t="str">
+        <v>22.22</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>